<commit_message>
Rerun w/ tables and flipped april
</commit_message>
<xml_diff>
--- a/tables/monthly_tables/detrended_covar/pc_timeseries.xlsx
+++ b/tables/monthly_tables/detrended_covar/pc_timeseries.xlsx
@@ -3451,464 +3451,464 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.9379418824767054</v>
+        <v>-0.9379418824767054</v>
       </c>
       <c r="B2" t="n">
-        <v>0.9981142189643205</v>
+        <v>-0.9981142189643205</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.135231486726972</v>
+        <v>0.135231486726972</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.989756536107737</v>
+        <v>-1.989756536107737</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.3990698167032556</v>
+        <v>0.3990698167032556</v>
       </c>
       <c r="C3" t="n">
-        <v>1.019506427428105</v>
+        <v>-1.019506427428105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.283035249349004</v>
+        <v>-2.283035249349004</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.015349917265753</v>
+        <v>1.015349917265753</v>
       </c>
       <c r="C4" t="n">
-        <v>2.069984685046169</v>
+        <v>-2.069984685046169</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.2432051194574877</v>
+        <v>-0.2432051194574877</v>
       </c>
       <c r="B5" t="n">
-        <v>1.789795008534226</v>
+        <v>-1.789795008534226</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.03350887289915692</v>
+        <v>0.03350887289915692</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-1.564922559882207</v>
+        <v>1.564922559882207</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1075143133582293</v>
+        <v>-0.1075143133582293</v>
       </c>
       <c r="C6" t="n">
-        <v>1.033216248590206</v>
+        <v>-1.033216248590206</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.5915821234800611</v>
+        <v>0.5915821234800611</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.418113492513833</v>
+        <v>1.418113492513833</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.04454184288948106</v>
+        <v>0.04454184288948106</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.4498865248077145</v>
+        <v>-0.4498865248077145</v>
       </c>
       <c r="B8" t="n">
-        <v>0.4123292656761517</v>
+        <v>-0.4123292656761517</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1350498843042796</v>
+        <v>-0.1350498843042796</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.324805862982201</v>
+        <v>0.324805862982201</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.2062690333678116</v>
+        <v>0.2062690333678116</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01495757599720605</v>
+        <v>-0.01495757599720605</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.321741224681151</v>
+        <v>-1.321741224681151</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.281471646664862</v>
+        <v>1.281471646664862</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.753094528759791</v>
+        <v>2.753094528759791</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-2.313371851409667</v>
+        <v>2.313371851409667</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.4385417719836302</v>
+        <v>0.4385417719836302</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2596497726273507</v>
+        <v>-0.2596497726273507</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-0.9310487085781692</v>
+        <v>0.9310487085781692</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6995994507136793</v>
+        <v>-0.6995994507136793</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.4940724219733666</v>
+        <v>0.4940724219733666</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>-1.557852069892796</v>
+        <v>1.557852069892796</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2095404142179527</v>
+        <v>-0.2095404142179527</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.6886329776137325</v>
+        <v>0.6886329776137325</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-1.328508942462656</v>
+        <v>1.328508942462656</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.7920089215660655</v>
+        <v>0.7920089215660655</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4185152982405994</v>
+        <v>-0.4185152982405994</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>-0.4026040147168604</v>
+        <v>0.4026040147168604</v>
       </c>
       <c r="B15" t="n">
-        <v>0.271585047359748</v>
+        <v>-0.271585047359748</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.8577242661568664</v>
+        <v>0.8577242661568664</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-0.5329922385187176</v>
+        <v>0.5329922385187176</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4457268448006911</v>
+        <v>-0.4457268448006911</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.050627658045595</v>
+        <v>2.050627658045595</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-0.8208718821958001</v>
+        <v>0.8208718821958001</v>
       </c>
       <c r="B17" t="n">
-        <v>0.06786116310002897</v>
+        <v>-0.06786116310002897</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.3836402018365507</v>
+        <v>0.3836402018365507</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-0.1136092078662349</v>
+        <v>0.1136092078662349</v>
       </c>
       <c r="B18" t="n">
-        <v>0.6769248431627432</v>
+        <v>-0.6769248431627432</v>
       </c>
       <c r="C18" t="n">
-        <v>2.894240697217266</v>
+        <v>-2.894240697217266</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.191727726845455</v>
+        <v>-1.191727726845455</v>
       </c>
       <c r="B19" t="n">
-        <v>0.6738732851996604</v>
+        <v>-0.6738732851996604</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.9762318091124472</v>
+        <v>0.9762318091124472</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.4257786999785476</v>
+        <v>-0.4257786999785476</v>
       </c>
       <c r="B20" t="n">
-        <v>2.134723655871648</v>
+        <v>-2.134723655871648</v>
       </c>
       <c r="C20" t="n">
-        <v>0.6377496575181012</v>
+        <v>-0.6377496575181012</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.9587010202456556</v>
+        <v>-0.9587010202456556</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.5238159317276025</v>
+        <v>0.5238159317276025</v>
       </c>
       <c r="C21" t="n">
-        <v>-1.669331108864544</v>
+        <v>1.669331108864544</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.6123246233279082</v>
+        <v>-0.6123246233279082</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.2457896478621069</v>
+        <v>0.2457896478621069</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.6619775256993357</v>
+        <v>0.6619775256993357</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>-0.9018137575379827</v>
+        <v>0.9018137575379827</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.6308314674323727</v>
+        <v>0.6308314674323727</v>
       </c>
       <c r="C23" t="n">
-        <v>0.6745220200244013</v>
+        <v>-0.6745220200244013</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>-0.4924392378652002</v>
+        <v>0.4924392378652002</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.2846610488850265</v>
+        <v>0.2846610488850265</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3405370338766295</v>
+        <v>-0.3405370338766295</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.2434002380260795</v>
+        <v>-0.2434002380260795</v>
       </c>
       <c r="B25" t="n">
-        <v>0.3359319260706006</v>
+        <v>-0.3359319260706006</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.2519400953248681</v>
+        <v>0.2519400953248681</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.137321627868126</v>
+        <v>-1.137321627868126</v>
       </c>
       <c r="B26" t="n">
-        <v>0.147055821339385</v>
+        <v>-0.147055821339385</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.5970806252660655</v>
+        <v>0.5970806252660655</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.3137826440732399</v>
+        <v>-0.3137826440732399</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.3238447425060131</v>
+        <v>0.3238447425060131</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.5257895068328952</v>
+        <v>0.5257895068328952</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-0.7048129120672425</v>
+        <v>0.7048129120672425</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.958113406837526</v>
+        <v>0.958113406837526</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.4872501673778654</v>
+        <v>0.4872501673778654</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-0.05106760556818061</v>
+        <v>0.05106760556818061</v>
       </c>
       <c r="B29" t="n">
-        <v>-1.414910971304106</v>
+        <v>1.414910971304106</v>
       </c>
       <c r="C29" t="n">
-        <v>0.3271001527115822</v>
+        <v>-0.3271001527115822</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>-0.9573739947674434</v>
+        <v>0.9573739947674434</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.07859037634517128</v>
+        <v>0.07859037634517128</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.03366855805788511</v>
+        <v>0.03366855805788511</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>-0.3062819115820858</v>
+        <v>0.3062819115820858</v>
       </c>
       <c r="B31" t="n">
-        <v>0.8863941227776366</v>
+        <v>-0.8863941227776366</v>
       </c>
       <c r="C31" t="n">
-        <v>0.2385755523066092</v>
+        <v>-0.2385755523066092</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.32522405568474</v>
+        <v>-0.32522405568474</v>
       </c>
       <c r="B32" t="n">
-        <v>0.7863875030953752</v>
+        <v>-0.7863875030953752</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1944601803131988</v>
+        <v>-0.1944601803131988</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.5337012620903346</v>
+        <v>-0.5337012620903346</v>
       </c>
       <c r="B33" t="n">
-        <v>-3.52005362894627</v>
+        <v>3.52005362894627</v>
       </c>
       <c r="C33" t="n">
-        <v>0.8042011625908574</v>
+        <v>-0.8042011625908574</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>-0.9096876241556664</v>
+        <v>0.9096876241556664</v>
       </c>
       <c r="B34" t="n">
-        <v>1.65338761711859</v>
+        <v>-1.65338761711859</v>
       </c>
       <c r="C34" t="n">
-        <v>0.9469256055685751</v>
+        <v>-0.9469256055685751</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-0.8241388182118641</v>
+        <v>0.8241388182118641</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.5184011801999162</v>
+        <v>0.5184011801999162</v>
       </c>
       <c r="C35" t="n">
-        <v>0.4594093988919764</v>
+        <v>-0.4594093988919764</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1.690483026277675</v>
+        <v>-1.690483026277675</v>
       </c>
       <c r="B36" t="n">
-        <v>0.4330798705356188</v>
+        <v>-0.4330798705356188</v>
       </c>
       <c r="C36" t="n">
-        <v>1.921870013232539</v>
+        <v>-1.921870013232539</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>-0.3843384014867079</v>
+        <v>0.3843384014867079</v>
       </c>
       <c r="B37" t="n">
-        <v>1.23618964464605</v>
+        <v>-1.23618964464605</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.7782918753424545</v>
+        <v>0.7782918753424545</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.837314922208571</v>
+        <v>-0.837314922208571</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.690457764773533</v>
+        <v>0.690457764773533</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.1737703468771779</v>
+        <v>0.1737703468771779</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-1.315069432800067</v>
+        <v>1.315069432800067</v>
       </c>
       <c r="B39" t="n">
-        <v>-0.937024763563819</v>
+        <v>0.937024763563819</v>
       </c>
       <c r="C39" t="n">
-        <v>0.6393954011389522</v>
+        <v>-0.6393954011389522</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.5539535771196941</v>
+        <v>-0.5539535771196941</v>
       </c>
       <c r="B40" t="n">
-        <v>0.1955404716414562</v>
+        <v>-0.1955404716414562</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.6852904367441137</v>
+        <v>0.6852904367441137</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.9384225241867921</v>
+        <v>-0.9384225241867921</v>
       </c>
       <c r="B41" t="n">
-        <v>1.083770128475629</v>
+        <v>-1.083770128475629</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.3536166242763129</v>
+        <v>0.3536166242763129</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.1459513074759024</v>
+        <v>-0.1459513074759024</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.2740922671165578</v>
+        <v>0.2740922671165578</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.4272528155174843</v>
+        <v>0.4272528155174843</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.1955393657392914</v>
+        <v>-0.1955393657392914</v>
       </c>
       <c r="B43" t="n">
-        <v>0.7060871809058121</v>
+        <v>-0.7060871809058121</v>
       </c>
       <c r="C43" t="n">
-        <v>0.03269898457035858</v>
+        <v>-0.03269898457035858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>